<commit_message>
Add extra pressure sensor model
</commit_message>
<xml_diff>
--- a/Sensors table.xlsx
+++ b/Sensors table.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>OIL_TEMP</t>
   </si>
@@ -43,13 +43,16 @@
   <si>
     <t>bar</t>
   </si>
+  <si>
+    <t>Oil_PRESSURE2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -128,9 +131,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -358,11 +361,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-456900784"/>
-        <c:axId val="-456914480"/>
+        <c:axId val="-1575357456"/>
+        <c:axId val="-1610988512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-456900784"/>
+        <c:axId val="-1575357456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -418,12 +421,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-456914480"/>
+        <c:crossAx val="-1610988512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-456914480"/>
+        <c:axId val="-1610988512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -479,7 +482,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-456900784"/>
+        <c:crossAx val="-1575357456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -789,11 +792,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-456858976"/>
-        <c:axId val="-460092384"/>
+        <c:axId val="-1610975152"/>
+        <c:axId val="-1610972672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-456858976"/>
+        <c:axId val="-1610975152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,12 +853,12 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-460092384"/>
+        <c:crossAx val="-1610972672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-460092384"/>
+        <c:axId val="-1610972672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -911,7 +914,360 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-456858976"/>
+        <c:crossAx val="-1610975152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ohm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$A$23:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$B$23:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>88.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>106.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>124.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>170.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>184.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1540374960"/>
+        <c:axId val="-1540389424"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1540374960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1540389424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1540389424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1540374960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1040,6 +1396,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1557,6 +1953,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2129,6 +3041,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2403,7 +3345,7 @@
   <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D26"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2671,6 +3613,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
       <c r="D21" s="5">
         <v>1.4</v>
       </c>
@@ -2678,7 +3623,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="D22" s="5">
         <v>1.2</v>
       </c>
@@ -2686,7 +3637,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2">
+        <v>10</v>
+      </c>
       <c r="D23" s="5">
         <v>1</v>
       </c>
@@ -2695,6 +3652,12 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1">
+        <v>31</v>
+      </c>
       <c r="D24" s="5">
         <v>0.8</v>
       </c>
@@ -2703,6 +3666,12 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>52</v>
+      </c>
       <c r="D25" s="5">
         <v>0.6</v>
       </c>
@@ -2711,6 +3680,12 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1">
+        <v>71</v>
+      </c>
       <c r="D26" s="5">
         <v>0.4</v>
       </c>
@@ -2719,69 +3694,111 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1">
+        <v>88</v>
+      </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1">
+        <v>106</v>
+      </c>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>6</v>
+      </c>
+      <c r="B29" s="1">
+        <v>124</v>
+      </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1">
+        <v>140</v>
+      </c>
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1">
+        <v>155</v>
+      </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>9</v>
+      </c>
+      <c r="B32" s="1">
+        <v>170</v>
+      </c>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>10</v>
+      </c>
+      <c r="B33" s="1">
+        <v>184</v>
+      </c>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.2">
@@ -2903,6 +3920,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>